<commit_message>
refactor: let the user choice a different directory for sheets
</commit_message>
<xml_diff>
--- a/Planilhas/10- Outubro Rating -.xlsx
+++ b/Planilhas/10- Outubro Rating -.xlsx
@@ -2696,7 +2696,7 @@
   <dimension ref="A1:K157"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2756,7 +2756,7 @@
         <v>11</v>
       </c>
       <c r="C2" s="13" t="n">
-        <v>19996389319</v>
+        <v>19992558897</v>
       </c>
       <c r="D2" s="14"/>
       <c r="E2" s="15" t="n">

</xml_diff>